<commit_message>
update data file after additional quality check
</commit_message>
<xml_diff>
--- a/data/raw_data/ManyPrimates Pilot Coding -kano.xlsx
+++ b/data/raw_data/ManyPrimates Pilot Coding -kano.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBohn/Work/ManyPrimates/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBohn/Work/ManyPrimates/ManyPrimates_pilot/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1979029A-BFA8-964D-8571-8251F0BC7C4C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72D260F-2694-7641-BF43-DCD7D685F925}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$T$433</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4478" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4496" uniqueCount="71">
   <si>
     <t>date</t>
   </si>
@@ -10660,8 +10660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E254" sqref="E254:E289"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R244" sqref="R244:R253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24714,6 +24714,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R245" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="246" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A246">
@@ -24768,6 +24771,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R246" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="247" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A247">
@@ -24822,6 +24828,9 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="R247" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="248" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A248">
@@ -24876,6 +24885,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R248" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="249" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A249">
@@ -24930,6 +24942,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R249" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="250" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A250">
@@ -24984,6 +24999,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R250" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="251" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A251">
@@ -25038,6 +25056,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R251" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="252" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A252">
@@ -25092,6 +25113,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R252" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="253" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A253">
@@ -25146,6 +25170,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="R253" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="254" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A254">
@@ -35220,6 +35247,9 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="R425" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="426" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A426">
@@ -35274,6 +35304,9 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="R426" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="427" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A427">
@@ -35328,6 +35361,9 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="R427" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="428" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A428">
@@ -35382,6 +35418,9 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="R428" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="429" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A429">
@@ -35436,6 +35475,9 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="R429" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="430" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A430">
@@ -35490,6 +35532,9 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="R430" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="431" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A431">
@@ -35544,6 +35589,9 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
+      <c r="R431" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="432" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A432">
@@ -35598,8 +35646,11 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="433" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R432" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="433" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A433">
         <v>20180328</v>
       </c>
@@ -35651,6 +35702,9 @@
       <c r="Q433">
         <f t="shared" si="6"/>
         <v>1</v>
+      </c>
+      <c r="R433" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>